<commit_message>
updated instructions & added April students, ran build
</commit_message>
<xml_diff>
--- a/src/data/test.xlsx
+++ b/src/data/test.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rickyz/Downloads/Graduation/src/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rickyz/Downloads/Graduation Jan 22/src/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEFE283A-AC49-0E48-A45D-7D9FCFA35565}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C40F1A5-CB98-9843-B1D6-2449C179835C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4140" yWindow="1380" windowWidth="19300" windowHeight="17400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="84">
   <si>
     <t>name</t>
   </si>
@@ -31,208 +31,250 @@
     <t>github</t>
   </si>
   <si>
-    <t>Abhishek Bornak</t>
-  </si>
-  <si>
-    <t>Agustin Zucca</t>
-  </si>
-  <si>
-    <t>Anthony Bronca</t>
-  </si>
-  <si>
-    <t>Anthony Lovern</t>
-  </si>
-  <si>
-    <t>Ara Sargsyan</t>
-  </si>
-  <si>
-    <t>Brendan Downing</t>
-  </si>
-  <si>
-    <t>Brian May</t>
-  </si>
-  <si>
-    <t>Briana Robinson</t>
-  </si>
-  <si>
-    <t>Celeste Winterton</t>
-  </si>
-  <si>
-    <t>Christopher (Chris) Threadgill</t>
-  </si>
-  <si>
-    <t>Darren Kong</t>
-  </si>
-  <si>
-    <t>David Forster</t>
-  </si>
-  <si>
-    <t>Elan Katz</t>
-  </si>
-  <si>
-    <t>Ethan Chen</t>
-  </si>
-  <si>
-    <t>Fang Yue</t>
-  </si>
-  <si>
-    <t>Frances Huang</t>
-  </si>
-  <si>
-    <t>Jingling Jin</t>
-  </si>
-  <si>
-    <t>Jonathan (Jon) Halquist</t>
-  </si>
-  <si>
-    <t>Jonathon Tufts</t>
-  </si>
-  <si>
-    <t>Joshua (Josh) Bautista</t>
-  </si>
-  <si>
-    <t>Kevin Bartolome</t>
-  </si>
-  <si>
-    <t>Lincoln Her</t>
-  </si>
-  <si>
-    <t>Maica Santos</t>
-  </si>
-  <si>
-    <t>Mark Osman</t>
-  </si>
-  <si>
-    <t>Mason Kogami</t>
-  </si>
-  <si>
-    <t>Mason Taylor</t>
-  </si>
-  <si>
-    <t>Noel Mutia</t>
-  </si>
-  <si>
-    <t>Paul-Eirik (Paul) Melhus</t>
-  </si>
-  <si>
-    <t>Philip (Kai) Seward</t>
-  </si>
-  <si>
-    <t>Sam Kramer</t>
-  </si>
-  <si>
-    <t>Sviatlana (Lana) Komar</t>
-  </si>
-  <si>
-    <t>Vee Alianza</t>
-  </si>
-  <si>
-    <t>Vernyoon Chao</t>
-  </si>
-  <si>
-    <t>Xiaowen Nie</t>
-  </si>
-  <si>
-    <t>starsabhi</t>
-  </si>
-  <si>
-    <t>AgustinZucca</t>
-  </si>
-  <si>
-    <t>AnthonyBronca</t>
-  </si>
-  <si>
-    <t>Amlovern</t>
-  </si>
-  <si>
-    <t>arasargsyan0622</t>
-  </si>
-  <si>
-    <t>Downster</t>
-  </si>
-  <si>
-    <t>brianmay2014</t>
-  </si>
-  <si>
-    <t>BriRob</t>
-  </si>
-  <si>
-    <t>celestewinterton</t>
-  </si>
-  <si>
-    <t>ChrisThreadgill</t>
-  </si>
-  <si>
-    <t>dkong1321</t>
-  </si>
-  <si>
-    <t>da5idf</t>
-  </si>
-  <si>
-    <t>otter23</t>
-  </si>
-  <si>
-    <t>ethanchen7</t>
-  </si>
-  <si>
-    <t>yuefang323</t>
-  </si>
-  <si>
-    <t>frances-y-h</t>
-  </si>
-  <si>
-    <t>ellen20</t>
-  </si>
-  <si>
-    <t>halquist</t>
-  </si>
-  <si>
-    <t>jonathontufts</t>
-  </si>
-  <si>
-    <t>jrbauti-09</t>
-  </si>
-  <si>
-    <t>Kxvin1</t>
-  </si>
-  <si>
-    <t>LincolnHer</t>
-  </si>
-  <si>
-    <t>itsmaica</t>
-  </si>
-  <si>
-    <t>thisismydisplay</t>
-  </si>
-  <si>
-    <t>MasonKogami</t>
-  </si>
-  <si>
-    <t>masontaylor7</t>
-  </si>
-  <si>
-    <t>leonphoenix21</t>
-  </si>
-  <si>
-    <t>pmelhus</t>
-  </si>
-  <si>
-    <t>kairality</t>
-  </si>
-  <si>
-    <t>samuelrkramer</t>
-  </si>
-  <si>
-    <t>lanakomar</t>
-  </si>
-  <si>
-    <t>vee-alianza</t>
-  </si>
-  <si>
-    <t>VernyoonChao98</t>
-  </si>
-  <si>
-    <t>xwnnie</t>
+    <t>Abel Tesfa</t>
+  </si>
+  <si>
+    <t>Allen Faughn</t>
+  </si>
+  <si>
+    <t>Anai (Anai (Amy)) Lopez</t>
+  </si>
+  <si>
+    <t>Andrew (Andy) Vallas</t>
+  </si>
+  <si>
+    <t>Angela (Angie) Maidt</t>
+  </si>
+  <si>
+    <t>Anthony Taylor</t>
+  </si>
+  <si>
+    <t>Brandon Flores</t>
+  </si>
+  <si>
+    <t>Christian Alcantara-Cayanan</t>
+  </si>
+  <si>
+    <t>Connor Burns</t>
+  </si>
+  <si>
+    <t>David Chung</t>
+  </si>
+  <si>
+    <t>David (Mag) Rivera</t>
+  </si>
+  <si>
+    <t>Edwin (Eddie) Lau</t>
+  </si>
+  <si>
+    <t>Elias Rodriguez</t>
+  </si>
+  <si>
+    <t>Ethan Browning</t>
+  </si>
+  <si>
+    <t>Isaac Diaz</t>
+  </si>
+  <si>
+    <t>Israel Arvizu</t>
+  </si>
+  <si>
+    <t>Jack Tran</t>
+  </si>
+  <si>
+    <t>Janie (Jay) Hutts</t>
+  </si>
+  <si>
+    <t>Jeffrey Kintner</t>
+  </si>
+  <si>
+    <t>Jesse Njoroge</t>
+  </si>
+  <si>
+    <t>Jiaqi (Jackie) Cheng</t>
+  </si>
+  <si>
+    <t>Jingjing Xu</t>
+  </si>
+  <si>
+    <t>Jingxun Yin</t>
+  </si>
+  <si>
+    <t>John Pham</t>
+  </si>
+  <si>
+    <t>John Voskuyl</t>
+  </si>
+  <si>
+    <t>Jonathan Kim</t>
+  </si>
+  <si>
+    <t>Josef (Niels) Griedel</t>
+  </si>
+  <si>
+    <t>Joshua (Josh) Salcido</t>
+  </si>
+  <si>
+    <t>Justin Stockton</t>
+  </si>
+  <si>
+    <t>Krishna Mulloth</t>
+  </si>
+  <si>
+    <t>Luis Sanchez-Porras</t>
+  </si>
+  <si>
+    <t>Matthew (Matty) Dickerson</t>
+  </si>
+  <si>
+    <t>Michael Dasch</t>
+  </si>
+  <si>
+    <t>Michael Presley</t>
+  </si>
+  <si>
+    <t>Mineh Gharabegi</t>
+  </si>
+  <si>
+    <t>Patrick Mcpherson</t>
+  </si>
+  <si>
+    <t>Rouben Ghambaryan</t>
+  </si>
+  <si>
+    <t>Tianyi Shao</t>
+  </si>
+  <si>
+    <t>Wing Nin (Ricky) Cheung</t>
+  </si>
+  <si>
+    <t>Xiangyou Wang</t>
+  </si>
+  <si>
+    <t>Zhiqi (Rena) Lin</t>
+  </si>
+  <si>
+    <t>abeltesfa</t>
+  </si>
+  <si>
+    <t>aFaughn</t>
+  </si>
+  <si>
+    <t>anailopez</t>
+  </si>
+  <si>
+    <t>vallas01</t>
+  </si>
+  <si>
+    <t>angmaidt</t>
+  </si>
+  <si>
+    <t>antt3</t>
+  </si>
+  <si>
+    <t>brandonflores647</t>
+  </si>
+  <si>
+    <t>Christian-AC</t>
+  </si>
+  <si>
+    <t>ConnorBurns1993</t>
+  </si>
+  <si>
+    <t>dchung007</t>
+  </si>
+  <si>
+    <t>Dave89rr</t>
+  </si>
+  <si>
+    <t>elabbit</t>
+  </si>
+  <si>
+    <t>bo-codes</t>
+  </si>
+  <si>
+    <t>eebrowning</t>
+  </si>
+  <si>
+    <t>Palillo10</t>
+  </si>
+  <si>
+    <t>israel-arvizu</t>
+  </si>
+  <si>
+    <t>jackmtran</t>
+  </si>
+  <si>
+    <t>jay-bean</t>
+  </si>
+  <si>
+    <t>jkintner25</t>
+  </si>
+  <si>
+    <t>jnjoroge13</t>
+  </si>
+  <si>
+    <t>jiaqicheng1998</t>
+  </si>
+  <si>
+    <t>FloraKho</t>
+  </si>
+  <si>
+    <t>jxyin0513</t>
+  </si>
+  <si>
+    <t>john0123456789</t>
+  </si>
+  <si>
+    <t>jvos415</t>
+  </si>
+  <si>
+    <t>KimJonathan426</t>
+  </si>
+  <si>
+    <t>jngriedel</t>
+  </si>
+  <si>
+    <t>joshsalcido</t>
+  </si>
+  <si>
+    <t>Justin-Stockton</t>
+  </si>
+  <si>
+    <t>kmulloth</t>
+  </si>
+  <si>
+    <t>stuffy-doll</t>
+  </si>
+  <si>
+    <t>MonkeyToji</t>
+  </si>
+  <si>
+    <t>MDasch22</t>
+  </si>
+  <si>
+    <t>mipresley23</t>
+  </si>
+  <si>
+    <t>Mineh222</t>
+  </si>
+  <si>
+    <t>Patricus</t>
+  </si>
+  <si>
+    <t>RoubenGh</t>
+  </si>
+  <si>
+    <t>tshao42</t>
+  </si>
+  <si>
+    <t>WingNinCheung</t>
+  </si>
+  <si>
+    <t>whatsup-world</t>
+  </si>
+  <si>
+    <t>ZhiqiLinn</t>
   </si>
 </sst>
 </file>
@@ -742,10 +784,11 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1101,10 +1144,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B35"/>
+  <dimension ref="A1:B42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1122,275 +1165,331 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" s="3" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="B36" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37" s="3" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="B37" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38" s="3" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="B38" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39" s="3" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" t="s">
+      <c r="B39" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A40" s="3" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" t="s">
+      <c r="B40" s="3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A41" s="3" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" t="s">
+      <c r="B41" s="3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A42" s="3" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>15</v>
-      </c>
-      <c r="B15" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>16</v>
-      </c>
-      <c r="B16" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>17</v>
-      </c>
-      <c r="B17" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>18</v>
-      </c>
-      <c r="B18" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>19</v>
-      </c>
-      <c r="B19" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>20</v>
-      </c>
-      <c r="B20" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>21</v>
-      </c>
-      <c r="B21" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>22</v>
-      </c>
-      <c r="B22" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>23</v>
-      </c>
-      <c r="B23" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>24</v>
-      </c>
-      <c r="B24" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>25</v>
-      </c>
-      <c r="B25" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>26</v>
-      </c>
-      <c r="B26" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>27</v>
-      </c>
-      <c r="B27" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>28</v>
-      </c>
-      <c r="B28" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>29</v>
-      </c>
-      <c r="B29" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>30</v>
-      </c>
-      <c r="B30" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>31</v>
-      </c>
-      <c r="B31" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>32</v>
-      </c>
-      <c r="B32" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>33</v>
-      </c>
-      <c r="B33" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>34</v>
-      </c>
-      <c r="B34" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>35</v>
-      </c>
-      <c r="B35" t="s">
-        <v>69</v>
+      <c r="B42" s="3" t="s">
+        <v>83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>